<commit_message>
updating doc resources in sandcastle projects
Workitems:
#1624552 SandCastle Web Site Support
#1631700 updating target documentation resources, and derivables
git-tfs-id: [https://payerportfolio.visualstudio.com/]$/USHC_AMER_US_ADU_HSP_Ua3/Source/Utilities/Dev;C1598824
</commit_message>
<xml_diff>
--- a/components/SandCastleServiceSpecification/Common/Derivables/LoggingOverview.xlsx
+++ b/components/SandCastleServiceSpecification/Common/Derivables/LoggingOverview.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C935E918-93E9-4E57-9FA8-1AB27547AF92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logging Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Modules Running in SCCT" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Modules Running in SCCT'!$A$1:$E$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Modules Running in SCCT'!$A$1:$D$15</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -143,149 +144,161 @@
     <t>Excerpt from the server : 10.163.58.68</t>
   </si>
   <si>
-    <t>Module Name</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>Drug Rebate</t>
   </si>
   <si>
-    <t>ready, published</t>
-  </si>
-  <si>
     <t>TPL Policy</t>
   </si>
   <si>
-    <t>ManagedCare</t>
-  </si>
-  <si>
     <t>Provider Management</t>
   </si>
   <si>
     <t>Task Management</t>
   </si>
   <si>
-    <t>ProgramIntegrity</t>
-  </si>
-  <si>
     <t>Administration</t>
   </si>
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>http://servicespecs.shared.mapshc.com/DrugRebate/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/TPLCase/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/TPL/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/ManagedCare/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/ProviderMgmt/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/TaskMgmt/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/MemberMgmt/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/ProgramIntegrity/19.1.64.2/HelpWeb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/Administration/19.1.64.2/helpweb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/FinancialManagement/19.1.64.2/helpweb/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/Administration/19.1.64.2/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/PlanMgmt/19.1.64.2/HelpWeb/CodeInformation/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/PlanMgmt/19.1.64.2/HelpWeb/Grouping/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/PlanMgmt/19.1.64.2/HelpWeb/RateSettings/Index.html</t>
-  </si>
-  <si>
-    <t>http://servicespecs.shared.mapshc.com/PlanMgmt/19.1.64.2/HelpWeb/RelatedInformation/Index.html</t>
-  </si>
-  <si>
-    <t>Services (BAS solution)</t>
-  </si>
-  <si>
     <t>TPL Case Tracking</t>
   </si>
   <si>
-    <t>Member Management</t>
-  </si>
-  <si>
     <t>Program Integrity</t>
   </si>
   <si>
-    <t>Finantial Management</t>
-  </si>
-  <si>
-    <t>DrugRebate</t>
-  </si>
-  <si>
-    <t>TPLCase</t>
-  </si>
-  <si>
-    <t>TPLPolicy</t>
-  </si>
-  <si>
-    <t>ProviderManagement</t>
-  </si>
-  <si>
-    <t>MemberManagement</t>
-  </si>
-  <si>
-    <t>TaskManagement</t>
-  </si>
-  <si>
-    <t>Code Information</t>
-  </si>
-  <si>
-    <t>Rate Settings</t>
-  </si>
-  <si>
-    <t>Related Information</t>
-  </si>
-  <si>
-    <t>Grouping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Management </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Administration </t>
-  </si>
-  <si>
-    <t>BroadCastMessage</t>
-  </si>
-  <si>
-    <t>Finantial</t>
+    <t>Financial Management</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Active Module</t>
+  </si>
+  <si>
+    <t>BAS Solution</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Source\Administration\Dev\BAS\BroadcastMessage\HP.HSP.UA3.Administration.BAS.BroadcastMessage.sln</t>
+  </si>
+  <si>
+    <t>Source\DrugRebate\Dev\BAS\DrugRebate\HP.HSP.UA3.DrugRebate.BAS.DrugRebate.sln</t>
+  </si>
+  <si>
+    <t>Source\FinancialManagement\Dev\BAS\FinancialManagementSvc\HP.HSP.UA3.FinancialManagement.BAS.FinancialManagementSvc.sln</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Source\Integration\Dev\BAS\Integration\HP.HSP.UA3.Integration.BAS.Integration.sln</t>
+  </si>
+  <si>
+    <t>Indentity Management</t>
+  </si>
+  <si>
+    <t>Source\IdentityManagement\Dev\BAS\User\HP.HSP.UA3.IdentityManagement.BAS.User.sln</t>
+  </si>
+  <si>
+    <t>Managed Care</t>
+  </si>
+  <si>
+    <t>Source\ManagedCare\Dev\BAS\ManagedCare\HP.HSP.UA3.ManagedCare.BAS.ManagedCare.sln</t>
+  </si>
+  <si>
+    <t>Plan Management</t>
+  </si>
+  <si>
+    <t>Source\PlanManagement\Dev\BAS\Grouping\HP.HSP.UA3.PlanManagement.BAS.Grouping.sln</t>
+  </si>
+  <si>
+    <t>Source\PlanManagement\Dev\BAS\RategSettings\HP.HSP.UA3.PlanManagement.BAS.RateSetting.sln</t>
+  </si>
+  <si>
+    <t>Source\PlanManagement\Dev\BAS\RelatedInformation\HP.HSP.UA3.PlanManagement.BAS.RelatedInformation.sln</t>
+  </si>
+  <si>
+    <t>Source\PlanManagement\Dev\BAS\CodeInformation\HP.HSP.UA3.PlanManagement.BAS.CodeInformation.sln</t>
+  </si>
+  <si>
+    <t>Provider Screening</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\CLIA\HP.HSP.UA3.Screening.BAS.CLIA.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\Credentials\HP.HSP.UA3.Screening.BAS.Credentials.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\DEA\HP.HSP.UA3.Screening.BAS.DEA.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\LEIE\HP.HSP.UA3.Screening.BAS.LEIESvc.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\MCSIS\HP.HSP.UA3.Screening.BAS.MCSIS.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\NPPES\HP.HSP.UA3.Screening.BAS.NPPES.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\PECOS\HP.HSP.UA3.Screening.BAS.PECOS.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\SAMCHECK\HP.HSP.UA3.Screening.BAS.SAMCheck.sln</t>
+  </si>
+  <si>
+    <t>Source\Screening\Dev\BAS\SSNDEATHMASTER\HP.HSP.UA3.SSNDeathMaster.BAS.SSDMF.sln</t>
+  </si>
+  <si>
+    <t>Provider Credentialing</t>
+  </si>
+  <si>
+    <t>Source\ProviderCredentialing\Dev\BAS\Audit\HP.HSP.UA3.ProviderCredentialing.BAS.Audit.sln</t>
+  </si>
+  <si>
+    <t>Source\ProviderCredentialing\Dev\BAS\FileManagement\HP.HSP.UA3.ProviderCredentialing.BAS.FileMgmt.sln</t>
+  </si>
+  <si>
+    <t>Source\ProviderCredentialing\Dev\BAS\ValidateCredentials\HP.HSP.UA3.ProviderCredentialing.BAS.ValCrdntls.sln</t>
+  </si>
+  <si>
+    <t>Provider Enrollment</t>
+  </si>
+  <si>
+    <t>Source\ProviderEnrollment\Dev\BAS\EnrollmentSvc\HP.HSP.UA3.ProviderEnrollment.BAS.EnrollmentSvc.sln</t>
+  </si>
+  <si>
+    <t>Source\ProgramIntegrity\Dev\BAS\ProgramIntegritySvc\HP.HSP.UA3.ProgramIntegrity.BAS.ProgramIntegritySvc.sln</t>
+  </si>
+  <si>
+    <t>Program Integrity Case Tracking</t>
+  </si>
+  <si>
+    <t>Source\ProgramIntegrityCT\Dev\BAS\CaseTracking\HP.HSP.UA3.ProgramIntegrityCT.BAS.CaseTracking.sln</t>
+  </si>
+  <si>
+    <t>Source\ProviderManagement\Dev\BAS\ProviderSvc\HP.HSP.UA3.ProviderManagement.BAS.ProviderSvc.sln</t>
+  </si>
+  <si>
+    <t>Source\TPLCaseTracking\Dev\BAS\CaseTracking\HP.HSP.UA3.TPLCaseTracking.BAS.CaseTracking.sln</t>
+  </si>
+  <si>
+    <t>Source\TPLPolicy\Dev\BAS\Policy\HP.HSP.UA3.TPLPolicy.BAS.Policy.sln</t>
+  </si>
+  <si>
+    <t>Source\TaskManagement\Dev\BAS\TaskManagement\HP.HSP.UA3.TaskManagement.BAS.TaskManagement.sln</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,14 +309,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -332,25 +337,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,7 +406,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -485,6 +514,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -520,6 +566,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -695,25 +758,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -733,7 +796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -753,7 +816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -773,7 +836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -793,7 +856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -813,7 +876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -833,7 +896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -853,7 +916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>10</v>
       </c>
@@ -873,7 +936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>11</v>
       </c>
@@ -893,7 +956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>12</v>
       </c>
@@ -913,7 +976,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>16</v>
       </c>
@@ -933,7 +996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>19</v>
       </c>
@@ -953,7 +1016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>20</v>
       </c>
@@ -973,19 +1036,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
       <c r="E17" s="2" t="s">
         <v>29</v>
@@ -997,7 +1060,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
       <c r="E18" t="s">
         <v>32</v>
@@ -1009,7 +1072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
       <c r="E19" t="s">
         <v>34</v>
@@ -1021,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
       <c r="E20" t="s">
         <v>36</v>
@@ -1033,17 +1096,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E23" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>40</v>
       </c>
@@ -1055,311 +1118,443 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="153" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="27.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="113.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>63</v>
+      <c r="C28" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E16"/>
-  <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1"/>
-    <hyperlink ref="E6" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="E3" r:id="rId5"/>
-    <hyperlink ref="E2" r:id="rId6"/>
-    <hyperlink ref="E13" r:id="rId7"/>
-    <hyperlink ref="E12" r:id="rId8"/>
-    <hyperlink ref="E14" r:id="rId9"/>
-    <hyperlink ref="E15" r:id="rId10"/>
-    <hyperlink ref="E16" r:id="rId11"/>
-    <hyperlink ref="E8" r:id="rId12"/>
-    <hyperlink ref="E9" r:id="rId13"/>
-    <hyperlink ref="E10" r:id="rId14"/>
-    <hyperlink ref="E11" r:id="rId15"/>
-  </hyperlinks>
+  <autoFilter ref="A1:D15" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>